<commit_message>
the login tests scripts are complete
</commit_message>
<xml_diff>
--- a/testing code/src/test/java/resources/data.xlsx
+++ b/testing code/src/test/java/resources/data.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\third year\first term\software engineering\NonLegit-Code\Testing\SeleniumWebTesting\src\test\java\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\third year\first term\software engineering\NonLegit-Code\Testing\testing code\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660C856C-FD20-455B-9756-66BF13F093AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03544FE-C670-4B4B-8B78-F135846816FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7968" yWindow="2016" windowWidth="11508" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="googleLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="googleForgetUserNamePassword" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -61,6 +63,24 @@
   </si>
   <si>
     <t>success</t>
+  </si>
+  <si>
+    <t>Abdo@1357</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>am0643794@gmail.com</t>
+  </si>
+  <si>
+    <t>testmohamed113@gmail.com</t>
+  </si>
+  <si>
+    <t>zskwnnrhdeoxlooo</t>
+  </si>
+  <si>
+    <t>castfer</t>
   </si>
 </sst>
 </file>
@@ -391,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -461,8 +481,8 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -470,11 +490,100 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1"/>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{AF90BA89-5B92-4490-AF7B-35B9F1ACC059}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{43692EEB-2EE2-4665-B0EF-5791C3BEC5CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA838388-DCFF-464E-A658-9A24039E03A1}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="F6:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="20.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.62890625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AD1F2BF1-008C-4BC2-8045-4001478CD8ED}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{46A904D8-5ADF-4A78-8C31-31F3EB35A53A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49BE28-889D-4A84-B44F-BEE00CA8BA48}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="24.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.62890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{76EB17C1-809E-44A4-BE45-C15D3F4249E2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
initial mobile base test
</commit_message>
<xml_diff>
--- a/testing code/src/test/java/resources/data.xlsx
+++ b/testing code/src/test/java/resources/data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\third year\first term\software engineering\NonLegit-Code\Testing\testing code\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03544FE-C670-4B4B-8B78-F135846816FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C3DAED-3B06-4D2E-ACCD-2E68C9D59AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginTestData" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -81,12 +81,25 @@
   </si>
   <si>
     <t>castfer</t>
+  </si>
+  <si>
+    <t>Nho4DGqEoxtXBi1</t>
+  </si>
+  <si>
+    <t>RdPS8xmcPF*.</t>
+  </si>
+  <si>
+    <t>eagermanipulation</t>
+  </si>
+  <si>
+    <t>abi3u1nkXd*.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,89 +422,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.89453125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.41796875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.62890625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1"/>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -513,15 +548,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.26171875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.62890625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -546,25 +581,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49BE28-889D-4A84-B44F-BEE00CA8BA48}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.89453125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.62890625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>0</v>
       </c>
     </row>
@@ -575,7 +610,7 @@
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
intial mobile base test
</commit_message>
<xml_diff>
--- a/testing code/src/test/java/resources/data.xlsx
+++ b/testing code/src/test/java/resources/data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\third year\first term\software engineering\NonLegit-Code\Testing\testing code\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03544FE-C670-4B4B-8B78-F135846816FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C3DAED-3B06-4D2E-ACCD-2E68C9D59AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginTestData" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -81,12 +81,25 @@
   </si>
   <si>
     <t>castfer</t>
+  </si>
+  <si>
+    <t>Nho4DGqEoxtXBi1</t>
+  </si>
+  <si>
+    <t>RdPS8xmcPF*.</t>
+  </si>
+  <si>
+    <t>eagermanipulation</t>
+  </si>
+  <si>
+    <t>abi3u1nkXd*.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,89 +422,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.89453125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.41796875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.62890625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1"/>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -513,15 +548,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.26171875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.62890625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -546,25 +581,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C49BE28-889D-4A84-B44F-BEE00CA8BA48}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.89453125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.62890625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>0</v>
       </c>
     </row>
@@ -575,7 +610,7 @@
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
version 1.2 from testing
</commit_message>
<xml_diff>
--- a/testing code/src/test/java/resources/data.xlsx
+++ b/testing code/src/test/java/resources/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\third year\first term\software engineering\NonLegit-Code\Testing\testing code\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C3DAED-3B06-4D2E-ACCD-2E68C9D59AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B9663B-E8AF-42B1-92E7-E96E70671DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -59,15 +59,9 @@
     <t>DELETE *</t>
   </si>
   <si>
-    <t>Immediate_Rhubarb_75</t>
-  </si>
-  <si>
     <t>success</t>
   </si>
   <si>
-    <t>Abdo@1357</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -83,23 +77,34 @@
     <t>castfer</t>
   </si>
   <si>
-    <t>Nho4DGqEoxtXBi1</t>
-  </si>
-  <si>
-    <t>RdPS8xmcPF*.</t>
-  </si>
-  <si>
-    <t>eagermanipulation</t>
-  </si>
-  <si>
-    <t>abi3u1nkXd*.</t>
+    <t>Fawzy</t>
+  </si>
+  <si>
+    <t>Aa123456*.</t>
+  </si>
+  <si>
+    <t>Aa_123456789_Aa</t>
+  </si>
+  <si>
+    <t>bola</t>
+  </si>
+  <si>
+    <t>3abkareem</t>
+  </si>
+  <si>
+    <t>zuksh</t>
+  </si>
+  <si>
+    <t>bolt</t>
+  </si>
+  <si>
+    <t>messi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,117 +427,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.89453125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.41796875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.62890625"/>
+    <col min="1" max="1" width="19.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="1"/>
-      <c r="C7" t="s" s="0">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s" s="0">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s" s="0">
-        <v>11</v>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{AF90BA89-5B92-4490-AF7B-35B9F1ACC059}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{43692EEB-2EE2-4665-B0EF-5791C3BEC5CE}"/>
+    <hyperlink ref="B6" r:id="rId2" display="Abdo@1357" xr:uid="{43692EEB-2EE2-4665-B0EF-5791C3BEC5CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -543,26 +574,26 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="F6:G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.26171875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.62890625"/>
+    <col min="1" max="1" width="20.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -587,31 +618,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.89453125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.62890625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="27.578125"/>
+    <col min="1" max="1" width="24.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.62890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>